<commit_message>
Esto es de los análisis
</commit_message>
<xml_diff>
--- a/Pruebas de Usuario/Analisis/Evaluación VR Mandos y Guantes (respuestas).xlsx
+++ b/Pruebas de Usuario/Analisis/Evaluación VR Mandos y Guantes (respuestas).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Cole\TFG\TFG-2324-InteraccionVR\Pruebas de Usuario\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Cole\4\Tfg\TFG-2324-InteraccionVR\Pruebas de Usuario\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D08B71-98DD-4856-8353-6E523D49D7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803E5745-8411-4A17-B96C-05E94EB47897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -18,17 +18,52 @@
     <sheet name="Hoja3" sheetId="4" r:id="rId3"/>
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="27" r:id="rId5"/>
-    <pivotCache cacheId="31" r:id="rId6"/>
-    <pivotCache cacheId="36" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="3" r:id="rId7"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="163">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -523,9 +558,6 @@
     <t>Usuario_31</t>
   </si>
   <si>
-    <t>Suma de ¿Qué facilidad tuviste para aprender a coger/soltar objetos?</t>
-  </si>
-  <si>
     <t>Etiquetas de fila</t>
   </si>
   <si>
@@ -535,10 +567,10 @@
     <t>Promedio de ¿Qué facilidad tuviste para aprender a coger/soltar objetos?</t>
   </si>
   <si>
-    <t>Etiquetas de columna</t>
-  </si>
-  <si>
     <t>Promedio de ¿Qué opinas de la sensación de agarrar objetos?, ¿la has sentido realista?</t>
+  </si>
+  <si>
+    <t>Cuenta de Edad</t>
   </si>
 </sst>
 </file>
@@ -587,11 +619,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1770,6 +1802,457 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Evaluación VR Mandos y Guantes (respuestas).xlsx]Hoja3!TablaDinámica7</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja3!$A$4:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja3!$B$4:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E358-40EC-8E0D-6C862CFFE1A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="926049311"/>
+        <c:axId val="926040671"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="926049311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="926040671"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="926040671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="926049311"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1811,6 +2294,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2856,6 +3379,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2918,6 +3944,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47E2C925-7220-D1AD-01D2-BD16A2C67A0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>937260</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>960120</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFD0DA2C-7F0A-1C71-B676-C5C058DE6C2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3014,7 +4081,20 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Edad" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="19" maxValue="52"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="19" maxValue="52" count="12">
+        <n v="22"/>
+        <n v="21"/>
+        <n v="19"/>
+        <n v="25"/>
+        <n v="20"/>
+        <n v="51"/>
+        <n v="52"/>
+        <n v="42"/>
+        <n v="24"/>
+        <n v="23"/>
+        <n v="33"/>
+        <n v="29"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Género" numFmtId="0">
       <sharedItems/>
@@ -3479,7 +4559,7 @@
   <r>
     <d v="2024-04-22T19:14:46"/>
     <s v="Usuario_01"/>
-    <n v="22"/>
+    <x v="0"/>
     <s v="Femenino"/>
     <s v="Grado universitario"/>
     <x v="0"/>
@@ -3511,7 +4591,7 @@
   <r>
     <d v="2024-04-22T20:04:16"/>
     <s v="Usuario_02"/>
-    <n v="21"/>
+    <x v="1"/>
     <s v="Femenino"/>
     <s v="Grado universitario"/>
     <x v="0"/>
@@ -3543,7 +4623,7 @@
   <r>
     <d v="2024-04-22T20:26:49"/>
     <s v="Usuario_03"/>
-    <n v="22"/>
+    <x v="0"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="1"/>
@@ -3575,7 +4655,7 @@
   <r>
     <d v="2024-04-23T11:52:00"/>
     <s v=" Usuario_04"/>
-    <n v="19"/>
+    <x v="2"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="2"/>
@@ -3607,7 +4687,7 @@
   <r>
     <d v="2024-04-23T12:15:31"/>
     <s v="Usuario_05"/>
-    <n v="25"/>
+    <x v="3"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="2"/>
@@ -3639,7 +4719,7 @@
   <r>
     <d v="2024-04-23T12:49:38"/>
     <s v="Usuario_06"/>
-    <n v="20"/>
+    <x v="4"/>
     <s v="Femenino"/>
     <s v="Grado universitario"/>
     <x v="3"/>
@@ -3671,7 +4751,7 @@
   <r>
     <d v="2024-04-23T18:50:27"/>
     <s v="Usuario_07"/>
-    <n v="51"/>
+    <x v="5"/>
     <s v="Femenino"/>
     <s v="Doctorado"/>
     <x v="0"/>
@@ -3703,7 +4783,7 @@
   <r>
     <d v="2024-04-23T19:26:58"/>
     <s v="Usuario_08"/>
-    <n v="22"/>
+    <x v="0"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="2"/>
@@ -3735,7 +4815,7 @@
   <r>
     <d v="2024-04-23T20:08:32"/>
     <s v="Usuario_09"/>
-    <n v="22"/>
+    <x v="0"/>
     <s v="Femenino"/>
     <s v="Grado universitario"/>
     <x v="2"/>
@@ -3767,7 +4847,7 @@
   <r>
     <d v="2024-04-24T10:36:32"/>
     <s v="Usuario_10"/>
-    <n v="52"/>
+    <x v="6"/>
     <s v="Masculino"/>
     <s v="Doctorado"/>
     <x v="3"/>
@@ -3799,7 +4879,7 @@
   <r>
     <d v="2024-04-24T11:19:23"/>
     <s v="Usuario_11"/>
-    <n v="21"/>
+    <x v="1"/>
     <s v="Femenino"/>
     <s v="Grado universitario"/>
     <x v="1"/>
@@ -3831,7 +4911,7 @@
   <r>
     <d v="2024-04-24T12:00:34"/>
     <s v="Usuario_12"/>
-    <n v="42"/>
+    <x v="7"/>
     <s v="Masculino"/>
     <s v="Doctorado"/>
     <x v="1"/>
@@ -3863,7 +4943,7 @@
   <r>
     <d v="2024-04-24T12:38:46"/>
     <s v="Usuario_13"/>
-    <n v="24"/>
+    <x v="8"/>
     <s v="Femenino"/>
     <s v="Grado universitario"/>
     <x v="2"/>
@@ -3895,7 +4975,7 @@
   <r>
     <d v="2024-04-24T13:06:59"/>
     <s v="Usuario_14"/>
-    <n v="24"/>
+    <x v="8"/>
     <s v="Femenino"/>
     <s v="Formación profesional"/>
     <x v="3"/>
@@ -3927,7 +5007,7 @@
   <r>
     <d v="2024-04-24T17:21:47"/>
     <s v="Usuario_15"/>
-    <n v="23"/>
+    <x v="9"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="0"/>
@@ -3959,7 +5039,7 @@
   <r>
     <d v="2024-04-24T19:06:24"/>
     <s v="Usuario_16"/>
-    <n v="23"/>
+    <x v="9"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="2"/>
@@ -3991,7 +5071,7 @@
   <r>
     <d v="2024-04-24T19:54:25"/>
     <s v="Usuario_17"/>
-    <n v="22"/>
+    <x v="0"/>
     <s v="Masculino"/>
     <s v="Bachillerato"/>
     <x v="2"/>
@@ -4023,7 +5103,7 @@
   <r>
     <d v="2024-04-24T20:20:59"/>
     <s v="Usuario_18"/>
-    <n v="22"/>
+    <x v="0"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="1"/>
@@ -4055,7 +5135,7 @@
   <r>
     <d v="2024-04-25T11:12:44"/>
     <s v="Usuario_19"/>
-    <n v="23"/>
+    <x v="9"/>
     <s v="No Binario"/>
     <s v="Grado universitario"/>
     <x v="2"/>
@@ -4087,7 +5167,7 @@
   <r>
     <d v="2024-04-25T12:03:15"/>
     <s v="Usuario_20"/>
-    <n v="22"/>
+    <x v="0"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="2"/>
@@ -4119,7 +5199,7 @@
   <r>
     <d v="2024-04-25T12:49:46"/>
     <s v="Usuario_21"/>
-    <n v="19"/>
+    <x v="2"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="2"/>
@@ -4151,7 +5231,7 @@
   <r>
     <d v="2024-04-25T13:04:22"/>
     <s v="Usuario_22"/>
-    <n v="33"/>
+    <x v="10"/>
     <s v="Masculino"/>
     <s v="Doctorado"/>
     <x v="3"/>
@@ -4183,7 +5263,7 @@
   <r>
     <d v="2024-04-25T19:27:51"/>
     <s v="Usuario_23"/>
-    <n v="22"/>
+    <x v="0"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="2"/>
@@ -4215,7 +5295,7 @@
   <r>
     <d v="2024-04-25T20:01:35"/>
     <s v="Usuario_24"/>
-    <n v="22"/>
+    <x v="0"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="1"/>
@@ -4247,7 +5327,7 @@
   <r>
     <d v="2024-04-26T22:53:34"/>
     <s v="Usuario_25"/>
-    <n v="20"/>
+    <x v="4"/>
     <s v="Femenino"/>
     <s v="Bachillerato"/>
     <x v="3"/>
@@ -4279,7 +5359,7 @@
   <r>
     <d v="2024-04-26T14:21:22"/>
     <s v="Usuario_26"/>
-    <n v="21"/>
+    <x v="1"/>
     <s v="Femenino"/>
     <s v="Grado universitario"/>
     <x v="1"/>
@@ -4311,7 +5391,7 @@
   <r>
     <d v="2024-04-26T14:46:50"/>
     <s v="Usuario_27"/>
-    <n v="21"/>
+    <x v="1"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="2"/>
@@ -4343,7 +5423,7 @@
   <r>
     <d v="2024-04-26T16:55:57"/>
     <s v="usuario_28"/>
-    <n v="24"/>
+    <x v="8"/>
     <s v="Masculino"/>
     <s v="Grado universitario"/>
     <x v="2"/>
@@ -4375,7 +5455,7 @@
   <r>
     <d v="2024-04-26T17:35:33"/>
     <s v="Usuario 29"/>
-    <n v="20"/>
+    <x v="4"/>
     <s v="No Binario"/>
     <s v="Grado universitario"/>
     <x v="1"/>
@@ -4407,7 +5487,7 @@
   <r>
     <d v="2024-04-26T18:53:01"/>
     <s v="Usuario_30"/>
-    <n v="25"/>
+    <x v="3"/>
     <s v="Masculino"/>
     <s v="Master universitario"/>
     <x v="4"/>
@@ -4439,7 +5519,7 @@
   <r>
     <d v="2024-04-26T18:58:06"/>
     <s v="Usuario_31"/>
-    <n v="29"/>
+    <x v="11"/>
     <s v="Masculino"/>
     <s v="Master universitario"/>
     <x v="0"/>
@@ -4472,7 +5552,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8E7A2468-9069-43EB-9D98-37B4999DBE0C}" name="TablaDinámica5" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8E7A2468-9069-43EB-9D98-37B4999DBE0C}" name="TablaDinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="A1:A2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="1">
     <pivotField dataField="1" showAll="0">
@@ -4519,7 +5599,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0AF10C2E-B595-4BE7-9384-9009CB2D9013}" name="TablaDinámica6" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0AF10C2E-B595-4BE7-9384-9009CB2D9013}" name="TablaDinámica6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:A2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -4571,15 +5651,31 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6ABA09A8-385D-4B5D-AA97-F9EB89D9765A}" name="TablaDinámica7" cacheId="36" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:F10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6ABA09A8-385D-4B5D-AA97-F9EB89D9765A}" name="TablaDinámica7" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="30">
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="13">
+        <item x="2"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField showAll="0">
       <items count="6">
         <item x="3"/>
         <item x="2"/>
@@ -4593,7 +5689,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
+    <pivotField showAll="0">
       <items count="5">
         <item x="2"/>
         <item x="3"/>
@@ -4623,9 +5719,9 @@
     <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="5"/>
+    <field x="2"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="13">
     <i>
       <x/>
     </i>
@@ -4641,33 +5737,66 @@
     <i>
       <x v="4"/>
     </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="10"/>
-  </colFields>
-  <colItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Suma de ¿Qué facilidad tuviste para aprender a coger/soltar objetos?" fld="10" baseField="0" baseItem="0"/>
+    <dataField name="Cuenta de Edad" fld="2" subtotal="count" baseField="2" baseItem="1"/>
   </dataFields>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -4884,19 +6013,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>4.225806451612903</v>
       </c>
     </row>
@@ -4914,20 +6043,20 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>3</v>
       </c>
     </row>
@@ -4939,157 +6068,287 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F66554E4-FB43-440F-8549-27384AC97EB2}">
-  <dimension ref="A3:F10"/>
+  <dimension ref="A3:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>162</v>
       </c>
+      <c r="D3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>19</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f>D4*E4</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>20</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F15" si="0">D5*E5</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>21</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>22</v>
+      </c>
+      <c r="B7" s="5">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>23</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>24</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>24</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>25</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>29</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>33</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>33</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>42</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>42</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>51</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>51</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>52</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>52</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>160</v>
+      <c r="B16" s="5">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16">
+        <v>31</v>
+      </c>
+      <c r="F16">
+        <f>SUM(F4:F15)/E16</f>
+        <v>25.096774193548388</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3">
-        <v>3</v>
-      </c>
-      <c r="D5" s="3">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3">
-        <v>5</v>
-      </c>
-      <c r="F5" s="3">
-        <v>20</v>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="e" cm="1">
+        <f t="array" ref="B18">desv</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3">
-        <v>3</v>
-      </c>
-      <c r="D6" s="3">
-        <v>24</v>
-      </c>
-      <c r="E6" s="3">
-        <v>30</v>
-      </c>
-      <c r="F6" s="3">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3">
-        <v>15</v>
-      </c>
-      <c r="F7" s="3">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="3">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3">
-        <v>3</v>
-      </c>
-      <c r="D9" s="3">
-        <v>4</v>
-      </c>
-      <c r="E9" s="3">
-        <v>10</v>
-      </c>
-      <c r="F9" s="3">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3">
-        <v>60</v>
-      </c>
-      <c r="E10" s="3">
-        <v>60</v>
-      </c>
-      <c r="F10" s="3">
-        <v>131</v>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>AVERAGE(A4:B15)</f>
+        <v>16.333333333333332</v>
+      </c>
+      <c r="B19" t="e" cm="1">
+        <f t="array" ref="B19">med</f>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5100,17 +6359,17 @@
   </sheetPr>
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="36" width="18.85546875" customWidth="1"/>
+    <col min="1" max="36" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5202,7 +6461,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45404.801918645833</v>
       </c>
@@ -5294,7 +6553,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45404.836290740743</v>
       </c>
@@ -5386,7 +6645,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45404.851952789351</v>
       </c>
@@ -5478,7 +6737,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45405.494442349533</v>
       </c>
@@ -5570,7 +6829,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45405.510771215282</v>
       </c>
@@ -5662,7 +6921,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45405.534464178243</v>
       </c>
@@ -5754,7 +7013,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45405.785035578709</v>
       </c>
@@ -5846,7 +7105,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45405.810392465282</v>
       </c>
@@ -5938,7 +7197,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45405.839254143517</v>
       </c>
@@ -6030,7 +7289,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45406.442031736107</v>
       </c>
@@ -6122,7 +7381,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45406.471798935185</v>
       </c>
@@ -6214,7 +7473,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45406.500394930554</v>
       </c>
@@ -6306,7 +7565,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45406.526924907404</v>
       </c>
@@ -6398,7 +7657,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45406.546513310182</v>
       </c>
@@ -6490,7 +7749,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45406.72346202546</v>
       </c>
@@ -6582,7 +7841,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45406.796109016199</v>
       </c>
@@ -6674,7 +7933,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45406.82945907407</v>
       </c>
@@ -6766,7 +8025,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45406.847907881944</v>
       </c>
@@ -6858,7 +8117,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45407.467180717591</v>
       </c>
@@ -6950,7 +8209,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45407.502251979167</v>
       </c>
@@ -7042,7 +8301,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45407.534555925929</v>
       </c>
@@ -7134,7 +8393,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45407.544693298609</v>
       </c>
@@ -7226,7 +8485,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45407.81100616898</v>
       </c>
@@ -7318,7 +8577,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45407.834437812504</v>
       </c>
@@ -7410,7 +8669,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45408.953869722223</v>
       </c>
@@ -7502,7 +8761,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45408.598172986109</v>
       </c>
@@ -7594,7 +8853,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45408.615854606483</v>
       </c>
@@ -7686,7 +8945,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45408.705520428237</v>
       </c>
@@ -7778,7 +9037,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45408.73302594907</v>
       </c>
@@ -7870,7 +9129,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45408.786822106485</v>
       </c>
@@ -7962,7 +9221,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45408.790345555557</v>
       </c>

</xml_diff>